<commit_message>
lossofsale added up date17
</commit_message>
<xml_diff>
--- a/data/lossofsale_sg_calicut.xlsx
+++ b/data/lossofsale_sg_calicut.xlsx
@@ -284,20 +284,20 @@
       </c>
       <c t="inlineStr" r="B3">
         <is>
-          <t xml:space="preserve">17-12-2025</t>
+          <t xml:space="preserve">13-12-2025</t>
         </is>
       </c>
       <c t="inlineStr" r="C3">
         <is>
-          <t xml:space="preserve">shahid</t>
+          <t xml:space="preserve">sachin</t>
         </is>
       </c>
       <c r="D3" s="65">
-        <v>9895177222</v>
+        <v>9895964853</v>
       </c>
       <c t="inlineStr" r="E3">
         <is>
-          <t xml:space="preserve">20-12-2025</t>
+          <t xml:space="preserve">30-12-2025</t>
         </is>
       </c>
       <c t="inlineStr" r="F3">
@@ -312,12 +312,12 @@
       </c>
       <c t="inlineStr" r="H3">
         <is>
-          <t xml:space="preserve">ENQUIRY</t>
+          <t xml:space="preserve">PRODUCT</t>
         </is>
       </c>
       <c t="inlineStr" r="I3">
         <is>
-          <t xml:space="preserve">ENQUIRY WITHOUT BRIDE/FAMILY</t>
+          <t xml:space="preserve">PRODUCT NOT AVAILABLE</t>
         </is>
       </c>
       <c t="inlineStr" r="J3">
@@ -327,7 +327,7 @@
       </c>
       <c t="inlineStr" r="K3">
         <is>
-          <t xml:space="preserve">JUST ENQUIRY NEED TO VISIT OTHER STORES</t>
+          <t xml:space="preserve">sky blue suit</t>
         </is>
       </c>
     </row>
@@ -337,16 +337,16 @@
       </c>
       <c t="inlineStr" r="B4">
         <is>
-          <t xml:space="preserve">17-12-2025</t>
+          <t xml:space="preserve">13-12-2025</t>
         </is>
       </c>
       <c t="inlineStr" r="C4">
         <is>
-          <t xml:space="preserve">salman</t>
+          <t xml:space="preserve">vignesh</t>
         </is>
       </c>
       <c r="D4" s="65">
-        <v>8129510839</v>
+        <v>8086490774</v>
       </c>
       <c t="inlineStr" r="E4">
         <is>
@@ -355,7 +355,7 @@
       </c>
       <c t="inlineStr" r="F4">
         <is>
-          <t xml:space="preserve">AKHIL K</t>
+          <t xml:space="preserve">MUHAMMED ROSHAN C V</t>
         </is>
       </c>
       <c t="inlineStr" r="G4">
@@ -380,7 +380,7 @@
       </c>
       <c t="inlineStr" r="K4">
         <is>
-          <t xml:space="preserve">revisit again</t>
+          <t xml:space="preserve">revist again within 2days</t>
         </is>
       </c>
     </row>
@@ -390,25 +390,25 @@
       </c>
       <c t="inlineStr" r="B5">
         <is>
-          <t xml:space="preserve">17-12-2025</t>
+          <t xml:space="preserve">13-12-2025</t>
         </is>
       </c>
       <c t="inlineStr" r="C5">
         <is>
-          <t xml:space="preserve">anjith</t>
+          <t xml:space="preserve">shani</t>
         </is>
       </c>
       <c r="D5" s="65">
-        <v>9995707815</v>
+        <v>8281980642</v>
       </c>
       <c t="inlineStr" r="E5">
         <is>
-          <t xml:space="preserve">21-01-2026</t>
+          <t xml:space="preserve">05-01-2026</t>
         </is>
       </c>
       <c t="inlineStr" r="F5">
         <is>
-          <t xml:space="preserve">MUHAMMED ROSHAN C V</t>
+          <t xml:space="preserve">SHAIKRIZWAN</t>
         </is>
       </c>
       <c t="inlineStr" r="G5">
@@ -433,7 +433,7 @@
       </c>
       <c t="inlineStr" r="K5">
         <is>
-          <t xml:space="preserve">need to visit other stores</t>
+          <t xml:space="preserve">need to visit other Store</t>
         </is>
       </c>
     </row>
@@ -443,25 +443,25 @@
       </c>
       <c t="inlineStr" r="B6">
         <is>
-          <t xml:space="preserve">17-12-2025</t>
+          <t xml:space="preserve">14-12-2025</t>
         </is>
       </c>
       <c t="inlineStr" r="C6">
         <is>
-          <t xml:space="preserve">amir</t>
+          <t xml:space="preserve">adarsh</t>
         </is>
       </c>
       <c r="D6" s="65">
-        <v>8089616979</v>
+        <v>7510945212</v>
       </c>
       <c t="inlineStr" r="E6">
         <is>
-          <t xml:space="preserve">27-12-2025</t>
+          <t xml:space="preserve">28-12-2025</t>
         </is>
       </c>
       <c t="inlineStr" r="F6">
         <is>
-          <t xml:space="preserve">AKHIL K</t>
+          <t xml:space="preserve">SHAIKRIZWAN</t>
         </is>
       </c>
       <c t="inlineStr" r="G6">
@@ -486,7 +486,7 @@
       </c>
       <c t="inlineStr" r="K6">
         <is>
-          <t xml:space="preserve">collection not okay</t>
+          <t xml:space="preserve">need to visit another store</t>
         </is>
       </c>
     </row>
@@ -496,25 +496,25 @@
       </c>
       <c t="inlineStr" r="B7">
         <is>
-          <t xml:space="preserve">17-12-2025</t>
+          <t xml:space="preserve">14-12-2025</t>
         </is>
       </c>
       <c t="inlineStr" r="C7">
         <is>
-          <t xml:space="preserve">favas</t>
+          <t xml:space="preserve">AMJAD</t>
         </is>
       </c>
       <c r="D7" s="65">
-        <v>9995242944</v>
+        <v>8281287445</v>
       </c>
       <c t="inlineStr" r="E7">
         <is>
-          <t xml:space="preserve">23-12-2025</t>
+          <t xml:space="preserve">25-01-2026</t>
         </is>
       </c>
       <c t="inlineStr" r="F7">
         <is>
-          <t xml:space="preserve">AKHIL K</t>
+          <t xml:space="preserve">SHAIKRIZWAN</t>
         </is>
       </c>
       <c t="inlineStr" r="G7">
@@ -524,12 +524,12 @@
       </c>
       <c t="inlineStr" r="H7">
         <is>
-          <t xml:space="preserve">PRODUCT</t>
+          <t xml:space="preserve">ENQUIRY</t>
         </is>
       </c>
       <c t="inlineStr" r="I7">
         <is>
-          <t xml:space="preserve">REQUIRED MODEL NOT AVAILABLE</t>
+          <t xml:space="preserve">ENQUIRY WITHOUT BRIDE/FAMILY</t>
         </is>
       </c>
       <c t="inlineStr" r="J7">
@@ -539,7 +539,7 @@
       </c>
       <c t="inlineStr" r="K7">
         <is>
-          <t xml:space="preserve">kurtha model asking</t>
+          <t xml:space="preserve">WILL VISIT WITH FAMILY MEMBERS</t>
         </is>
       </c>
     </row>
@@ -549,48 +549,578 @@
       </c>
       <c t="inlineStr" r="B8">
         <is>
+          <t xml:space="preserve">14-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C8">
+        <is>
+          <t xml:space="preserve">sudin</t>
+        </is>
+      </c>
+      <c r="D8" s="65">
+        <v>7012152016</v>
+      </c>
+      <c t="inlineStr" r="E8">
+        <is>
+          <t xml:space="preserve">04-01-2026</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F8">
+        <is>
+          <t xml:space="preserve">SHAIKRIZWAN</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G8">
+        <is>
+          <t xml:space="preserve">Loss</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="H8">
+        <is>
+          <t xml:space="preserve">ENQUIRY</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="I8">
+        <is>
+          <t xml:space="preserve">Enquiry for Relative/Friend</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J8">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="K8">
+        <is>
+          <t xml:space="preserve">revisit again</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="65">
+        <v>7</v>
+      </c>
+      <c t="inlineStr" r="B9">
+        <is>
+          <t xml:space="preserve">14-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C9">
+        <is>
+          <t xml:space="preserve">abu</t>
+        </is>
+      </c>
+      <c r="D9" s="65">
+        <v>9633673890</v>
+      </c>
+      <c t="inlineStr" r="E9">
+        <is>
+          <t xml:space="preserve">21-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F9">
+        <is>
+          <t xml:space="preserve">SHAIKRIZWAN</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G9">
+        <is>
+          <t xml:space="preserve">Loss</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="H9">
+        <is>
+          <t xml:space="preserve">ENQUIRY</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="I9">
+        <is>
+          <t xml:space="preserve">ENQUIRY WITHOUT BRIDE/FAMILY</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J9">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="K9">
+        <is>
+          <t xml:space="preserve">need to visit another store</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="65">
+        <v>8</v>
+      </c>
+      <c t="inlineStr" r="B10">
+        <is>
+          <t xml:space="preserve">15-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C10">
+        <is>
+          <t xml:space="preserve">shahhul</t>
+        </is>
+      </c>
+      <c r="D10" s="65">
+        <v>7902726831</v>
+      </c>
+      <c t="inlineStr" r="E10">
+        <is>
+          <t xml:space="preserve">15-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F10">
+        <is>
+          <t xml:space="preserve">AKHIL K</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G10">
+        <is>
+          <t xml:space="preserve">Loss</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="H10">
+        <is>
+          <t xml:space="preserve">PRODUCT</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="I10">
+        <is>
+          <t xml:space="preserve">PRODUCT NOT AVAILABLE</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J10">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="K10">
+        <is>
+          <t xml:space="preserve">bangala black collection not okay</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="65">
+        <v>9</v>
+      </c>
+      <c t="inlineStr" r="B11">
+        <is>
+          <t xml:space="preserve">15-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C11">
+        <is>
+          <t xml:space="preserve">SINAN</t>
+        </is>
+      </c>
+      <c r="D11" s="65">
+        <v>7994796857</v>
+      </c>
+      <c t="inlineStr" r="E11">
+        <is>
+          <t xml:space="preserve">13-01-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F11">
+        <is>
+          <t xml:space="preserve">MUHAMMED ROSHAN C V</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G11">
+        <is>
+          <t xml:space="preserve">Loss</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="H11">
+        <is>
+          <t xml:space="preserve">PRODUCT</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="I11">
+        <is>
+          <t xml:space="preserve">REQUIRED MODEL NOT AVAILABLE</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J11">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="K11">
+        <is>
+          <t xml:space="preserve">IW MODEL NOT OKAY</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="65">
+        <v>10</v>
+      </c>
+      <c t="inlineStr" r="B12">
+        <is>
+          <t xml:space="preserve">16-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C12">
+        <is>
+          <t xml:space="preserve">shafeeq</t>
+        </is>
+      </c>
+      <c r="D12" s="65">
+        <v>9072804076</v>
+      </c>
+      <c t="inlineStr" r="E12">
+        <is>
+          <t xml:space="preserve">12-01-2026</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F12">
+        <is>
+          <t xml:space="preserve">SHAIKRIZWAN</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G12">
+        <is>
+          <t xml:space="preserve">Loss</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="H12">
+        <is>
+          <t xml:space="preserve">PRODUCT</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="I12">
+        <is>
+          <t xml:space="preserve">PRODUCT NOT AVAILABLE</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J12">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="K12">
+        <is>
+          <t xml:space="preserve">GOLDEN FULL WORK SUIT</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="65">
+        <v>11</v>
+      </c>
+      <c t="inlineStr" r="B13">
+        <is>
           <t xml:space="preserve">17-12-2025</t>
         </is>
       </c>
-      <c t="inlineStr" r="C8">
+      <c t="inlineStr" r="C13">
+        <is>
+          <t xml:space="preserve">shahid</t>
+        </is>
+      </c>
+      <c r="D13" s="65">
+        <v>9895177222</v>
+      </c>
+      <c t="inlineStr" r="E13">
+        <is>
+          <t xml:space="preserve">20-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F13">
+        <is>
+          <t xml:space="preserve">MUHAMMED ROSHAN C V</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G13">
+        <is>
+          <t xml:space="preserve">Loss</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="H13">
+        <is>
+          <t xml:space="preserve">ENQUIRY</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="I13">
+        <is>
+          <t xml:space="preserve">ENQUIRY WITHOUT BRIDE/FAMILY</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J13">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="K13">
+        <is>
+          <t xml:space="preserve">JUST ENQUIRY NEED TO VISIT OTHER STORES</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="65">
+        <v>12</v>
+      </c>
+      <c t="inlineStr" r="B14">
+        <is>
+          <t xml:space="preserve">17-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C14">
+        <is>
+          <t xml:space="preserve">salman</t>
+        </is>
+      </c>
+      <c r="D14" s="65">
+        <v>8129510839</v>
+      </c>
+      <c t="inlineStr" r="E14">
+        <is>
+          <t xml:space="preserve">02-01-2026</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F14">
+        <is>
+          <t xml:space="preserve">AKHIL K</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G14">
+        <is>
+          <t xml:space="preserve">Loss</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="H14">
+        <is>
+          <t xml:space="preserve">ENQUIRY</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="I14">
+        <is>
+          <t xml:space="preserve">ENQUIRY WITHOUT BRIDE/FAMILY</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J14">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="K14">
+        <is>
+          <t xml:space="preserve">revisit again</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="65">
+        <v>13</v>
+      </c>
+      <c t="inlineStr" r="B15">
+        <is>
+          <t xml:space="preserve">17-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C15">
+        <is>
+          <t xml:space="preserve">anjith</t>
+        </is>
+      </c>
+      <c r="D15" s="65">
+        <v>9995707815</v>
+      </c>
+      <c t="inlineStr" r="E15">
+        <is>
+          <t xml:space="preserve">21-01-2026</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F15">
+        <is>
+          <t xml:space="preserve">MUHAMMED ROSHAN C V</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G15">
+        <is>
+          <t xml:space="preserve">Loss</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="H15">
+        <is>
+          <t xml:space="preserve">ENQUIRY</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="I15">
+        <is>
+          <t xml:space="preserve">ENQUIRY WITHOUT BRIDE/FAMILY</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J15">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="K15">
+        <is>
+          <t xml:space="preserve">need to visit other stores</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="65">
+        <v>14</v>
+      </c>
+      <c t="inlineStr" r="B16">
+        <is>
+          <t xml:space="preserve">17-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C16">
+        <is>
+          <t xml:space="preserve">amir</t>
+        </is>
+      </c>
+      <c r="D16" s="65">
+        <v>8089616979</v>
+      </c>
+      <c t="inlineStr" r="E16">
+        <is>
+          <t xml:space="preserve">27-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F16">
+        <is>
+          <t xml:space="preserve">AKHIL K</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G16">
+        <is>
+          <t xml:space="preserve">Loss</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="H16">
+        <is>
+          <t xml:space="preserve">ENQUIRY</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="I16">
+        <is>
+          <t xml:space="preserve">ENQUIRY WITHOUT TRIAL</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J16">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="K16">
+        <is>
+          <t xml:space="preserve">collection not okay</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="65">
+        <v>15</v>
+      </c>
+      <c t="inlineStr" r="B17">
+        <is>
+          <t xml:space="preserve">17-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C17">
+        <is>
+          <t xml:space="preserve">favas</t>
+        </is>
+      </c>
+      <c r="D17" s="65">
+        <v>9995242944</v>
+      </c>
+      <c t="inlineStr" r="E17">
+        <is>
+          <t xml:space="preserve">23-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F17">
+        <is>
+          <t xml:space="preserve">AKHIL K</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G17">
+        <is>
+          <t xml:space="preserve">Loss</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="H17">
+        <is>
+          <t xml:space="preserve">PRODUCT</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="I17">
+        <is>
+          <t xml:space="preserve">REQUIRED MODEL NOT AVAILABLE</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J17">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="K17">
+        <is>
+          <t xml:space="preserve">kurtha model asking</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="65">
+        <v>16</v>
+      </c>
+      <c t="inlineStr" r="B18">
+        <is>
+          <t xml:space="preserve">17-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C18">
         <is>
           <t xml:space="preserve">sarath</t>
         </is>
       </c>
-      <c r="D8" s="65">
+      <c r="D18" s="65">
         <v>9633808138</v>
       </c>
-      <c t="inlineStr" r="E8">
+      <c t="inlineStr" r="E18">
         <is>
           <t xml:space="preserve">11-01-2026</t>
         </is>
       </c>
-      <c t="inlineStr" r="F8">
+      <c t="inlineStr" r="F18">
         <is>
           <t xml:space="preserve">AKHIL K</t>
         </is>
       </c>
-      <c t="inlineStr" r="G8">
-        <is>
-          <t xml:space="preserve">Loss</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="H8">
+      <c t="inlineStr" r="G18">
+        <is>
+          <t xml:space="preserve">Loss</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="H18">
         <is>
           <t xml:space="preserve">ENQUIRY</t>
         </is>
       </c>
-      <c t="inlineStr" r="I8">
+      <c t="inlineStr" r="I18">
         <is>
           <t xml:space="preserve">Enquiry for Relative/Friend</t>
         </is>
       </c>
-      <c t="inlineStr" r="J8">
-        <is>
-          <t xml:space="preserve">-</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="K8">
+      <c t="inlineStr" r="J18">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="K18">
         <is>
           <t xml:space="preserve">revisit again</t>
         </is>

</xml_diff>

<commit_message>
fix(return-sync): rectify defect in return API synchronization process
- corrected return API data mapping and processing logic
- resolved sync failures causing incomplete return records
- ensured consistent ingestion during automated and manual sync runs
</commit_message>
<xml_diff>
--- a/data/lossofsale_sg_calicut.xlsx
+++ b/data/lossofsale_sg_calicut.xlsx
@@ -208,8 +208,8 @@
     <col min="5" max="5" width="17.55" customWidth="1"/>
     <col min="6" max="6" width="25.650000000000002" customWidth="1"/>
     <col min="7" max="7" width="8.100000000000001" customWidth="1"/>
-    <col min="8" max="8" width="10.8" customWidth="1"/>
-    <col min="9" max="9" width="37.800000000000004" customWidth="1"/>
+    <col min="8" max="8" width="32.400000000000006" customWidth="1"/>
+    <col min="9" max="9" width="39.150000000000006" customWidth="1"/>
     <col min="10" max="10" width="16.200000000000003" customWidth="1"/>
     <col min="11" max="11" width="52.650000000000006" customWidth="1"/>
   </cols>
@@ -284,25 +284,25 @@
       </c>
       <c t="inlineStr" r="B3">
         <is>
-          <t xml:space="preserve">13-12-2025</t>
+          <t xml:space="preserve">10-12-2025</t>
         </is>
       </c>
       <c t="inlineStr" r="C3">
         <is>
-          <t xml:space="preserve">sachin</t>
+          <t xml:space="preserve">afnas</t>
         </is>
       </c>
       <c r="D3" s="65">
-        <v>9895964853</v>
+        <v>8943277213</v>
       </c>
       <c t="inlineStr" r="E3">
         <is>
-          <t xml:space="preserve">30-12-2025</t>
+          <t xml:space="preserve">04-01-2026</t>
         </is>
       </c>
       <c t="inlineStr" r="F3">
         <is>
-          <t xml:space="preserve">MUHAMMED ROSHAN C V</t>
+          <t xml:space="preserve">AKHIL K</t>
         </is>
       </c>
       <c t="inlineStr" r="G3">
@@ -327,7 +327,7 @@
       </c>
       <c t="inlineStr" r="K3">
         <is>
-          <t xml:space="preserve">sky blue suit</t>
+          <t xml:space="preserve">black 3ps collection not satisfied</t>
         </is>
       </c>
     </row>
@@ -337,22 +337,22 @@
       </c>
       <c t="inlineStr" r="B4">
         <is>
+          <t xml:space="preserve">10-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C4">
+        <is>
+          <t xml:space="preserve">riyas</t>
+        </is>
+      </c>
+      <c r="D4" s="65">
+        <v>9846361668</v>
+      </c>
+      <c t="inlineStr" r="E4">
+        <is>
           <t xml:space="preserve">13-12-2025</t>
         </is>
       </c>
-      <c t="inlineStr" r="C4">
-        <is>
-          <t xml:space="preserve">vignesh</t>
-        </is>
-      </c>
-      <c r="D4" s="65">
-        <v>8086490774</v>
-      </c>
-      <c t="inlineStr" r="E4">
-        <is>
-          <t xml:space="preserve">02-01-2026</t>
-        </is>
-      </c>
       <c t="inlineStr" r="F4">
         <is>
           <t xml:space="preserve">MUHAMMED ROSHAN C V</t>
@@ -365,12 +365,12 @@
       </c>
       <c t="inlineStr" r="H4">
         <is>
-          <t xml:space="preserve">ENQUIRY</t>
+          <t xml:space="preserve">PRODUCT</t>
         </is>
       </c>
       <c t="inlineStr" r="I4">
         <is>
-          <t xml:space="preserve">ENQUIRY WITHOUT BRIDE/FAMILY</t>
+          <t xml:space="preserve">PRODUCT NOT AVAILABLE</t>
         </is>
       </c>
       <c t="inlineStr" r="J4">
@@ -380,7 +380,7 @@
       </c>
       <c t="inlineStr" r="K4">
         <is>
-          <t xml:space="preserve">revist again within 2days</t>
+          <t xml:space="preserve">need boot cut fit suit</t>
         </is>
       </c>
     </row>
@@ -390,20 +390,20 @@
       </c>
       <c t="inlineStr" r="B5">
         <is>
-          <t xml:space="preserve">13-12-2025</t>
+          <t xml:space="preserve">11-12-2025</t>
         </is>
       </c>
       <c t="inlineStr" r="C5">
         <is>
-          <t xml:space="preserve">shani</t>
+          <t xml:space="preserve">shammu</t>
         </is>
       </c>
       <c r="D5" s="65">
-        <v>8281980642</v>
+        <v>9544243153</v>
       </c>
       <c t="inlineStr" r="E5">
         <is>
-          <t xml:space="preserve">05-01-2026</t>
+          <t xml:space="preserve">30-12-2025</t>
         </is>
       </c>
       <c t="inlineStr" r="F5">
@@ -433,7 +433,7 @@
       </c>
       <c t="inlineStr" r="K5">
         <is>
-          <t xml:space="preserve">need to visit other Store</t>
+          <t xml:space="preserve">revisit again</t>
         </is>
       </c>
     </row>
@@ -443,20 +443,20 @@
       </c>
       <c t="inlineStr" r="B6">
         <is>
-          <t xml:space="preserve">14-12-2025</t>
+          <t xml:space="preserve">11-12-2025</t>
         </is>
       </c>
       <c t="inlineStr" r="C6">
         <is>
-          <t xml:space="preserve">adarsh</t>
+          <t xml:space="preserve">basim</t>
         </is>
       </c>
       <c r="D6" s="65">
-        <v>7510945212</v>
+        <v>9847490366</v>
       </c>
       <c t="inlineStr" r="E6">
         <is>
-          <t xml:space="preserve">28-12-2025</t>
+          <t xml:space="preserve">11-01-2026</t>
         </is>
       </c>
       <c t="inlineStr" r="F6">
@@ -476,7 +476,7 @@
       </c>
       <c t="inlineStr" r="I6">
         <is>
-          <t xml:space="preserve">ENQUIRY WITHOUT TRIAL</t>
+          <t xml:space="preserve">ENQUIRY WITHOUT BRIDE/FAMILY</t>
         </is>
       </c>
       <c t="inlineStr" r="J6">
@@ -486,7 +486,7 @@
       </c>
       <c t="inlineStr" r="K6">
         <is>
-          <t xml:space="preserve">need to visit another store</t>
+          <t xml:space="preserve">revisit again later</t>
         </is>
       </c>
     </row>
@@ -496,25 +496,25 @@
       </c>
       <c t="inlineStr" r="B7">
         <is>
-          <t xml:space="preserve">14-12-2025</t>
+          <t xml:space="preserve">11-12-2025</t>
         </is>
       </c>
       <c t="inlineStr" r="C7">
         <is>
-          <t xml:space="preserve">AMJAD</t>
+          <t xml:space="preserve">raneesh</t>
         </is>
       </c>
       <c r="D7" s="65">
-        <v>8281287445</v>
+        <v>9656318689</v>
       </c>
       <c t="inlineStr" r="E7">
         <is>
-          <t xml:space="preserve">25-01-2026</t>
+          <t xml:space="preserve">11-12-2025</t>
         </is>
       </c>
       <c t="inlineStr" r="F7">
         <is>
-          <t xml:space="preserve">SHAIKRIZWAN</t>
+          <t xml:space="preserve">AKHIL K</t>
         </is>
       </c>
       <c t="inlineStr" r="G7">
@@ -524,12 +524,12 @@
       </c>
       <c t="inlineStr" r="H7">
         <is>
-          <t xml:space="preserve">ENQUIRY</t>
+          <t xml:space="preserve">PRODUCT</t>
         </is>
       </c>
       <c t="inlineStr" r="I7">
         <is>
-          <t xml:space="preserve">ENQUIRY WITHOUT BRIDE/FAMILY</t>
+          <t xml:space="preserve">REQUIRED DESIGN NOT AVAILABLE</t>
         </is>
       </c>
       <c t="inlineStr" r="J7">
@@ -539,7 +539,7 @@
       </c>
       <c t="inlineStr" r="K7">
         <is>
-          <t xml:space="preserve">WILL VISIT WITH FAMILY MEMBERS</t>
+          <t xml:space="preserve">2ps sky blue</t>
         </is>
       </c>
     </row>
@@ -549,20 +549,20 @@
       </c>
       <c t="inlineStr" r="B8">
         <is>
-          <t xml:space="preserve">14-12-2025</t>
+          <t xml:space="preserve">11-12-2025</t>
         </is>
       </c>
       <c t="inlineStr" r="C8">
         <is>
-          <t xml:space="preserve">sudin</t>
+          <t xml:space="preserve">nafal</t>
         </is>
       </c>
       <c r="D8" s="65">
-        <v>7012152016</v>
+        <v>9946907552</v>
       </c>
       <c t="inlineStr" r="E8">
         <is>
-          <t xml:space="preserve">04-01-2026</t>
+          <t xml:space="preserve">28-12-2025</t>
         </is>
       </c>
       <c t="inlineStr" r="F8">
@@ -577,12 +577,12 @@
       </c>
       <c t="inlineStr" r="H8">
         <is>
-          <t xml:space="preserve">ENQUIRY</t>
+          <t xml:space="preserve">PRODUCT</t>
         </is>
       </c>
       <c t="inlineStr" r="I8">
         <is>
-          <t xml:space="preserve">Enquiry for Relative/Friend</t>
+          <t xml:space="preserve">PRODUCT NOT AVAILABLE</t>
         </is>
       </c>
       <c t="inlineStr" r="J8">
@@ -592,7 +592,7 @@
       </c>
       <c t="inlineStr" r="K8">
         <is>
-          <t xml:space="preserve">revisit again</t>
+          <t xml:space="preserve">off white suit</t>
         </is>
       </c>
     </row>
@@ -602,25 +602,25 @@
       </c>
       <c t="inlineStr" r="B9">
         <is>
-          <t xml:space="preserve">14-12-2025</t>
+          <t xml:space="preserve">11-12-2025</t>
         </is>
       </c>
       <c t="inlineStr" r="C9">
         <is>
-          <t xml:space="preserve">abu</t>
+          <t xml:space="preserve">rameesh</t>
         </is>
       </c>
       <c r="D9" s="65">
-        <v>9633673890</v>
+        <v>9633990445</v>
       </c>
       <c t="inlineStr" r="E9">
         <is>
-          <t xml:space="preserve">21-12-2025</t>
+          <t xml:space="preserve">10-01-2026</t>
         </is>
       </c>
       <c t="inlineStr" r="F9">
         <is>
-          <t xml:space="preserve">SHAIKRIZWAN</t>
+          <t xml:space="preserve">AKHIL K</t>
         </is>
       </c>
       <c t="inlineStr" r="G9">
@@ -630,12 +630,12 @@
       </c>
       <c t="inlineStr" r="H9">
         <is>
-          <t xml:space="preserve">ENQUIRY</t>
+          <t xml:space="preserve">PRODUCT</t>
         </is>
       </c>
       <c t="inlineStr" r="I9">
         <is>
-          <t xml:space="preserve">ENQUIRY WITHOUT BRIDE/FAMILY</t>
+          <t xml:space="preserve">REQUIRED DESIGN NOT AVAILABLE</t>
         </is>
       </c>
       <c t="inlineStr" r="J9">
@@ -645,7 +645,7 @@
       </c>
       <c t="inlineStr" r="K9">
         <is>
-          <t xml:space="preserve">need to visit another store</t>
+          <t xml:space="preserve">collection not okay</t>
         </is>
       </c>
     </row>
@@ -655,25 +655,25 @@
       </c>
       <c t="inlineStr" r="B10">
         <is>
-          <t xml:space="preserve">15-12-2025</t>
+          <t xml:space="preserve">12-12-2025</t>
         </is>
       </c>
       <c t="inlineStr" r="C10">
         <is>
-          <t xml:space="preserve">shahhul</t>
+          <t xml:space="preserve">nihad</t>
         </is>
       </c>
       <c r="D10" s="65">
-        <v>7902726831</v>
+        <v>9995874916</v>
       </c>
       <c t="inlineStr" r="E10">
         <is>
-          <t xml:space="preserve">15-12-2025</t>
+          <t xml:space="preserve">12-12-2025</t>
         </is>
       </c>
       <c t="inlineStr" r="F10">
         <is>
-          <t xml:space="preserve">AKHIL K</t>
+          <t xml:space="preserve">PUNARTH K</t>
         </is>
       </c>
       <c t="inlineStr" r="G10">
@@ -688,7 +688,7 @@
       </c>
       <c t="inlineStr" r="I10">
         <is>
-          <t xml:space="preserve">PRODUCT NOT AVAILABLE</t>
+          <t xml:space="preserve">REQUIRED MODEL NOT AVAILABLE</t>
         </is>
       </c>
       <c t="inlineStr" r="J10">
@@ -698,7 +698,7 @@
       </c>
       <c t="inlineStr" r="K10">
         <is>
-          <t xml:space="preserve">bangala black collection not okay</t>
+          <t xml:space="preserve">COLLECTION NOT OKAY</t>
         </is>
       </c>
     </row>
@@ -708,20 +708,20 @@
       </c>
       <c t="inlineStr" r="B11">
         <is>
-          <t xml:space="preserve">15-12-2025</t>
+          <t xml:space="preserve">12-12-2025</t>
         </is>
       </c>
       <c t="inlineStr" r="C11">
         <is>
-          <t xml:space="preserve">SINAN</t>
+          <t xml:space="preserve">shreyas</t>
         </is>
       </c>
       <c r="D11" s="65">
-        <v>7994796857</v>
+        <v>7994208854</v>
       </c>
       <c t="inlineStr" r="E11">
         <is>
-          <t xml:space="preserve">13-01-2025</t>
+          <t xml:space="preserve">28-12-2025</t>
         </is>
       </c>
       <c t="inlineStr" r="F11">
@@ -736,12 +736,12 @@
       </c>
       <c t="inlineStr" r="H11">
         <is>
-          <t xml:space="preserve">PRODUCT</t>
+          <t xml:space="preserve">ENQUIRY</t>
         </is>
       </c>
       <c t="inlineStr" r="I11">
         <is>
-          <t xml:space="preserve">REQUIRED MODEL NOT AVAILABLE</t>
+          <t xml:space="preserve">ENQUIRY WITHOUT BRIDE/FAMILY</t>
         </is>
       </c>
       <c t="inlineStr" r="J11">
@@ -751,7 +751,7 @@
       </c>
       <c t="inlineStr" r="K11">
         <is>
-          <t xml:space="preserve">IW MODEL NOT OKAY</t>
+          <t xml:space="preserve">custumer need to visit other store</t>
         </is>
       </c>
     </row>
@@ -761,25 +761,25 @@
       </c>
       <c t="inlineStr" r="B12">
         <is>
-          <t xml:space="preserve">16-12-2025</t>
+          <t xml:space="preserve">13-12-2025</t>
         </is>
       </c>
       <c t="inlineStr" r="C12">
         <is>
-          <t xml:space="preserve">shafeeq</t>
+          <t xml:space="preserve">sachin</t>
         </is>
       </c>
       <c r="D12" s="65">
-        <v>9072804076</v>
+        <v>9895964853</v>
       </c>
       <c t="inlineStr" r="E12">
         <is>
-          <t xml:space="preserve">12-01-2026</t>
+          <t xml:space="preserve">30-12-2025</t>
         </is>
       </c>
       <c t="inlineStr" r="F12">
         <is>
-          <t xml:space="preserve">SHAIKRIZWAN</t>
+          <t xml:space="preserve">MUHAMMED ROSHAN C V</t>
         </is>
       </c>
       <c t="inlineStr" r="G12">
@@ -804,7 +804,7 @@
       </c>
       <c t="inlineStr" r="K12">
         <is>
-          <t xml:space="preserve">GOLDEN FULL WORK SUIT</t>
+          <t xml:space="preserve">sky blue suit</t>
         </is>
       </c>
     </row>
@@ -814,20 +814,20 @@
       </c>
       <c t="inlineStr" r="B13">
         <is>
-          <t xml:space="preserve">17-12-2025</t>
+          <t xml:space="preserve">13-12-2025</t>
         </is>
       </c>
       <c t="inlineStr" r="C13">
         <is>
-          <t xml:space="preserve">shahid</t>
+          <t xml:space="preserve">vignesh</t>
         </is>
       </c>
       <c r="D13" s="65">
-        <v>9895177222</v>
+        <v>8086490774</v>
       </c>
       <c t="inlineStr" r="E13">
         <is>
-          <t xml:space="preserve">20-12-2025</t>
+          <t xml:space="preserve">02-01-2026</t>
         </is>
       </c>
       <c t="inlineStr" r="F13">
@@ -857,7 +857,7 @@
       </c>
       <c t="inlineStr" r="K13">
         <is>
-          <t xml:space="preserve">JUST ENQUIRY NEED TO VISIT OTHER STORES</t>
+          <t xml:space="preserve">revist again within 2days</t>
         </is>
       </c>
     </row>
@@ -867,25 +867,25 @@
       </c>
       <c t="inlineStr" r="B14">
         <is>
-          <t xml:space="preserve">17-12-2025</t>
+          <t xml:space="preserve">13-12-2025</t>
         </is>
       </c>
       <c t="inlineStr" r="C14">
         <is>
-          <t xml:space="preserve">salman</t>
+          <t xml:space="preserve">shani</t>
         </is>
       </c>
       <c r="D14" s="65">
-        <v>8129510839</v>
+        <v>8281980642</v>
       </c>
       <c t="inlineStr" r="E14">
         <is>
-          <t xml:space="preserve">02-01-2026</t>
+          <t xml:space="preserve">05-01-2026</t>
         </is>
       </c>
       <c t="inlineStr" r="F14">
         <is>
-          <t xml:space="preserve">AKHIL K</t>
+          <t xml:space="preserve">SHAIKRIZWAN</t>
         </is>
       </c>
       <c t="inlineStr" r="G14">
@@ -910,7 +910,7 @@
       </c>
       <c t="inlineStr" r="K14">
         <is>
-          <t xml:space="preserve">revisit again</t>
+          <t xml:space="preserve">need to visit other Store</t>
         </is>
       </c>
     </row>
@@ -920,25 +920,25 @@
       </c>
       <c t="inlineStr" r="B15">
         <is>
-          <t xml:space="preserve">17-12-2025</t>
+          <t xml:space="preserve">14-12-2025</t>
         </is>
       </c>
       <c t="inlineStr" r="C15">
         <is>
-          <t xml:space="preserve">anjith</t>
+          <t xml:space="preserve">adarsh</t>
         </is>
       </c>
       <c r="D15" s="65">
-        <v>9995707815</v>
+        <v>7510945212</v>
       </c>
       <c t="inlineStr" r="E15">
         <is>
-          <t xml:space="preserve">21-01-2026</t>
+          <t xml:space="preserve">28-12-2025</t>
         </is>
       </c>
       <c t="inlineStr" r="F15">
         <is>
-          <t xml:space="preserve">MUHAMMED ROSHAN C V</t>
+          <t xml:space="preserve">SHAIKRIZWAN</t>
         </is>
       </c>
       <c t="inlineStr" r="G15">
@@ -953,7 +953,7 @@
       </c>
       <c t="inlineStr" r="I15">
         <is>
-          <t xml:space="preserve">ENQUIRY WITHOUT BRIDE/FAMILY</t>
+          <t xml:space="preserve">ENQUIRY WITHOUT TRIAL</t>
         </is>
       </c>
       <c t="inlineStr" r="J15">
@@ -963,7 +963,7 @@
       </c>
       <c t="inlineStr" r="K15">
         <is>
-          <t xml:space="preserve">need to visit other stores</t>
+          <t xml:space="preserve">need to visit another store</t>
         </is>
       </c>
     </row>
@@ -973,25 +973,25 @@
       </c>
       <c t="inlineStr" r="B16">
         <is>
-          <t xml:space="preserve">17-12-2025</t>
+          <t xml:space="preserve">14-12-2025</t>
         </is>
       </c>
       <c t="inlineStr" r="C16">
         <is>
-          <t xml:space="preserve">amir</t>
+          <t xml:space="preserve">AMJAD</t>
         </is>
       </c>
       <c r="D16" s="65">
-        <v>8089616979</v>
+        <v>8281287445</v>
       </c>
       <c t="inlineStr" r="E16">
         <is>
-          <t xml:space="preserve">27-12-2025</t>
+          <t xml:space="preserve">25-01-2026</t>
         </is>
       </c>
       <c t="inlineStr" r="F16">
         <is>
-          <t xml:space="preserve">AKHIL K</t>
+          <t xml:space="preserve">SHAIKRIZWAN</t>
         </is>
       </c>
       <c t="inlineStr" r="G16">
@@ -1006,7 +1006,7 @@
       </c>
       <c t="inlineStr" r="I16">
         <is>
-          <t xml:space="preserve">ENQUIRY WITHOUT TRIAL</t>
+          <t xml:space="preserve">ENQUIRY WITHOUT BRIDE/FAMILY</t>
         </is>
       </c>
       <c t="inlineStr" r="J16">
@@ -1016,7 +1016,7 @@
       </c>
       <c t="inlineStr" r="K16">
         <is>
-          <t xml:space="preserve">collection not okay</t>
+          <t xml:space="preserve">WILL VISIT WITH FAMILY MEMBERS</t>
         </is>
       </c>
     </row>
@@ -1026,25 +1026,25 @@
       </c>
       <c t="inlineStr" r="B17">
         <is>
-          <t xml:space="preserve">17-12-2025</t>
+          <t xml:space="preserve">14-12-2025</t>
         </is>
       </c>
       <c t="inlineStr" r="C17">
         <is>
-          <t xml:space="preserve">favas</t>
+          <t xml:space="preserve">sudin</t>
         </is>
       </c>
       <c r="D17" s="65">
-        <v>9995242944</v>
+        <v>7012152016</v>
       </c>
       <c t="inlineStr" r="E17">
         <is>
-          <t xml:space="preserve">23-12-2025</t>
+          <t xml:space="preserve">04-01-2026</t>
         </is>
       </c>
       <c t="inlineStr" r="F17">
         <is>
-          <t xml:space="preserve">AKHIL K</t>
+          <t xml:space="preserve">SHAIKRIZWAN</t>
         </is>
       </c>
       <c t="inlineStr" r="G17">
@@ -1054,12 +1054,12 @@
       </c>
       <c t="inlineStr" r="H17">
         <is>
-          <t xml:space="preserve">PRODUCT</t>
+          <t xml:space="preserve">ENQUIRY</t>
         </is>
       </c>
       <c t="inlineStr" r="I17">
         <is>
-          <t xml:space="preserve">REQUIRED MODEL NOT AVAILABLE</t>
+          <t xml:space="preserve">Enquiry for Relative/Friend</t>
         </is>
       </c>
       <c t="inlineStr" r="J17">
@@ -1069,7 +1069,7 @@
       </c>
       <c t="inlineStr" r="K17">
         <is>
-          <t xml:space="preserve">kurtha model asking</t>
+          <t xml:space="preserve">revisit again</t>
         </is>
       </c>
     </row>
@@ -1079,50 +1079,1375 @@
       </c>
       <c t="inlineStr" r="B18">
         <is>
+          <t xml:space="preserve">14-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C18">
+        <is>
+          <t xml:space="preserve">abu</t>
+        </is>
+      </c>
+      <c r="D18" s="65">
+        <v>9633673890</v>
+      </c>
+      <c t="inlineStr" r="E18">
+        <is>
+          <t xml:space="preserve">21-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F18">
+        <is>
+          <t xml:space="preserve">SHAIKRIZWAN</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G18">
+        <is>
+          <t xml:space="preserve">Loss</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="H18">
+        <is>
+          <t xml:space="preserve">ENQUIRY</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="I18">
+        <is>
+          <t xml:space="preserve">ENQUIRY WITHOUT BRIDE/FAMILY</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J18">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="K18">
+        <is>
+          <t xml:space="preserve">need to visit another store</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="65">
+        <v>17</v>
+      </c>
+      <c t="inlineStr" r="B19">
+        <is>
+          <t xml:space="preserve">15-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C19">
+        <is>
+          <t xml:space="preserve">shahhul</t>
+        </is>
+      </c>
+      <c r="D19" s="65">
+        <v>7902726831</v>
+      </c>
+      <c t="inlineStr" r="E19">
+        <is>
+          <t xml:space="preserve">15-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F19">
+        <is>
+          <t xml:space="preserve">AKHIL K</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G19">
+        <is>
+          <t xml:space="preserve">Loss</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="H19">
+        <is>
+          <t xml:space="preserve">PRODUCT</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="I19">
+        <is>
+          <t xml:space="preserve">PRODUCT NOT AVAILABLE</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J19">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="K19">
+        <is>
+          <t xml:space="preserve">bangala black collection not okay</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="65">
+        <v>18</v>
+      </c>
+      <c t="inlineStr" r="B20">
+        <is>
+          <t xml:space="preserve">15-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C20">
+        <is>
+          <t xml:space="preserve">SINAN</t>
+        </is>
+      </c>
+      <c r="D20" s="65">
+        <v>7994796857</v>
+      </c>
+      <c t="inlineStr" r="E20">
+        <is>
+          <t xml:space="preserve">13-01-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F20">
+        <is>
+          <t xml:space="preserve">MUHAMMED ROSHAN C V</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G20">
+        <is>
+          <t xml:space="preserve">Loss</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="H20">
+        <is>
+          <t xml:space="preserve">PRODUCT</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="I20">
+        <is>
+          <t xml:space="preserve">REQUIRED MODEL NOT AVAILABLE</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J20">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="K20">
+        <is>
+          <t xml:space="preserve">IW MODEL NOT OKAY</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="65">
+        <v>19</v>
+      </c>
+      <c t="inlineStr" r="B21">
+        <is>
+          <t xml:space="preserve">16-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C21">
+        <is>
+          <t xml:space="preserve">shafeeq</t>
+        </is>
+      </c>
+      <c r="D21" s="65">
+        <v>9072804076</v>
+      </c>
+      <c t="inlineStr" r="E21">
+        <is>
+          <t xml:space="preserve">12-01-2026</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F21">
+        <is>
+          <t xml:space="preserve">SHAIKRIZWAN</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G21">
+        <is>
+          <t xml:space="preserve">Loss</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="H21">
+        <is>
+          <t xml:space="preserve">PRODUCT</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="I21">
+        <is>
+          <t xml:space="preserve">PRODUCT NOT AVAILABLE</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J21">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="K21">
+        <is>
+          <t xml:space="preserve">GOLDEN FULL WORK SUIT</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="65">
+        <v>20</v>
+      </c>
+      <c t="inlineStr" r="B22">
+        <is>
           <t xml:space="preserve">17-12-2025</t>
         </is>
       </c>
-      <c t="inlineStr" r="C18">
+      <c t="inlineStr" r="C22">
+        <is>
+          <t xml:space="preserve">shahid</t>
+        </is>
+      </c>
+      <c r="D22" s="65">
+        <v>9895177222</v>
+      </c>
+      <c t="inlineStr" r="E22">
+        <is>
+          <t xml:space="preserve">20-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F22">
+        <is>
+          <t xml:space="preserve">MUHAMMED ROSHAN C V</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G22">
+        <is>
+          <t xml:space="preserve">Loss</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="H22">
+        <is>
+          <t xml:space="preserve">ENQUIRY</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="I22">
+        <is>
+          <t xml:space="preserve">ENQUIRY WITHOUT BRIDE/FAMILY</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J22">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="K22">
+        <is>
+          <t xml:space="preserve">JUST ENQUIRY NEED TO VISIT OTHER STORES</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="65">
+        <v>21</v>
+      </c>
+      <c t="inlineStr" r="B23">
+        <is>
+          <t xml:space="preserve">17-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C23">
+        <is>
+          <t xml:space="preserve">salman</t>
+        </is>
+      </c>
+      <c r="D23" s="65">
+        <v>8129510839</v>
+      </c>
+      <c t="inlineStr" r="E23">
+        <is>
+          <t xml:space="preserve">02-01-2026</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F23">
+        <is>
+          <t xml:space="preserve">AKHIL K</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G23">
+        <is>
+          <t xml:space="preserve">Loss</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="H23">
+        <is>
+          <t xml:space="preserve">ENQUIRY</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="I23">
+        <is>
+          <t xml:space="preserve">ENQUIRY WITHOUT BRIDE/FAMILY</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J23">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="K23">
+        <is>
+          <t xml:space="preserve">revisit again</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="65">
+        <v>22</v>
+      </c>
+      <c t="inlineStr" r="B24">
+        <is>
+          <t xml:space="preserve">17-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C24">
+        <is>
+          <t xml:space="preserve">anjith</t>
+        </is>
+      </c>
+      <c r="D24" s="65">
+        <v>9995707815</v>
+      </c>
+      <c t="inlineStr" r="E24">
+        <is>
+          <t xml:space="preserve">21-01-2026</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F24">
+        <is>
+          <t xml:space="preserve">MUHAMMED ROSHAN C V</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G24">
+        <is>
+          <t xml:space="preserve">Loss</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="H24">
+        <is>
+          <t xml:space="preserve">ENQUIRY</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="I24">
+        <is>
+          <t xml:space="preserve">ENQUIRY WITHOUT BRIDE/FAMILY</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J24">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="K24">
+        <is>
+          <t xml:space="preserve">need to visit other stores</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="65">
+        <v>23</v>
+      </c>
+      <c t="inlineStr" r="B25">
+        <is>
+          <t xml:space="preserve">17-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C25">
+        <is>
+          <t xml:space="preserve">amir</t>
+        </is>
+      </c>
+      <c r="D25" s="65">
+        <v>8089616979</v>
+      </c>
+      <c t="inlineStr" r="E25">
+        <is>
+          <t xml:space="preserve">27-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F25">
+        <is>
+          <t xml:space="preserve">AKHIL K</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G25">
+        <is>
+          <t xml:space="preserve">Loss</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="H25">
+        <is>
+          <t xml:space="preserve">ENQUIRY</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="I25">
+        <is>
+          <t xml:space="preserve">ENQUIRY WITHOUT TRIAL</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J25">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="K25">
+        <is>
+          <t xml:space="preserve">collection not okay</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="65">
+        <v>24</v>
+      </c>
+      <c t="inlineStr" r="B26">
+        <is>
+          <t xml:space="preserve">17-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C26">
+        <is>
+          <t xml:space="preserve">favas</t>
+        </is>
+      </c>
+      <c r="D26" s="65">
+        <v>9995242944</v>
+      </c>
+      <c t="inlineStr" r="E26">
+        <is>
+          <t xml:space="preserve">23-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F26">
+        <is>
+          <t xml:space="preserve">AKHIL K</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G26">
+        <is>
+          <t xml:space="preserve">Loss</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="H26">
+        <is>
+          <t xml:space="preserve">PRODUCT</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="I26">
+        <is>
+          <t xml:space="preserve">REQUIRED MODEL NOT AVAILABLE</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J26">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="K26">
+        <is>
+          <t xml:space="preserve">kurtha model asking</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="65">
+        <v>25</v>
+      </c>
+      <c t="inlineStr" r="B27">
+        <is>
+          <t xml:space="preserve">17-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C27">
         <is>
           <t xml:space="preserve">sarath</t>
         </is>
       </c>
-      <c r="D18" s="65">
+      <c r="D27" s="65">
         <v>9633808138</v>
       </c>
-      <c t="inlineStr" r="E18">
+      <c t="inlineStr" r="E27">
         <is>
           <t xml:space="preserve">11-01-2026</t>
         </is>
       </c>
-      <c t="inlineStr" r="F18">
+      <c t="inlineStr" r="F27">
         <is>
           <t xml:space="preserve">AKHIL K</t>
         </is>
       </c>
-      <c t="inlineStr" r="G18">
-        <is>
-          <t xml:space="preserve">Loss</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="H18">
+      <c t="inlineStr" r="G27">
+        <is>
+          <t xml:space="preserve">Loss</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="H27">
         <is>
           <t xml:space="preserve">ENQUIRY</t>
         </is>
       </c>
-      <c t="inlineStr" r="I18">
+      <c t="inlineStr" r="I27">
         <is>
           <t xml:space="preserve">Enquiry for Relative/Friend</t>
         </is>
       </c>
-      <c t="inlineStr" r="J18">
-        <is>
-          <t xml:space="preserve">-</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="K18">
+      <c t="inlineStr" r="J27">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="K27">
         <is>
           <t xml:space="preserve">revisit again</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="65">
+        <v>26</v>
+      </c>
+      <c t="inlineStr" r="B28">
+        <is>
+          <t xml:space="preserve">18-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C28">
+        <is>
+          <t xml:space="preserve">Junaid</t>
+        </is>
+      </c>
+      <c r="D28" s="65">
+        <v>8592072580</v>
+      </c>
+      <c t="inlineStr" r="E28">
+        <is>
+          <t xml:space="preserve">20-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F28">
+        <is>
+          <t xml:space="preserve">AKHIL K</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G28">
+        <is>
+          <t xml:space="preserve">Loss</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="H28">
+        <is>
+          <t xml:space="preserve">PRODUCT</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="I28">
+        <is>
+          <t xml:space="preserve">REQUIRED DESIGN NOT AVAILABLE</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J28">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="K28">
+        <is>
+          <t xml:space="preserve">not satisfied with collections</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="65">
+        <v>27</v>
+      </c>
+      <c t="inlineStr" r="B29">
+        <is>
+          <t xml:space="preserve">18-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C29">
+        <is>
+          <t xml:space="preserve">Salam</t>
+        </is>
+      </c>
+      <c r="D29" s="65">
+        <v>9847638049</v>
+      </c>
+      <c t="inlineStr" r="E29">
+        <is>
+          <t xml:space="preserve">25-01-2026</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F29">
+        <is>
+          <t xml:space="preserve">AKHIL K</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G29">
+        <is>
+          <t xml:space="preserve">Loss</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="H29">
+        <is>
+          <t xml:space="preserve">ENQUIRY</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="I29">
+        <is>
+          <t xml:space="preserve">ENQUIRY WITHOUT BRIDE/FAMILY</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J29">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="K29">
+        <is>
+          <t xml:space="preserve">not confirmed revisit again</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="65">
+        <v>28</v>
+      </c>
+      <c t="inlineStr" r="B30">
+        <is>
+          <t xml:space="preserve">19-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C30">
+        <is>
+          <t xml:space="preserve">numan</t>
+        </is>
+      </c>
+      <c r="D30" s="65">
+        <v>8606549212</v>
+      </c>
+      <c t="inlineStr" r="E30">
+        <is>
+          <t xml:space="preserve">21-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F30">
+        <is>
+          <t xml:space="preserve">MUHAMMED ROSHAN C V</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G30">
+        <is>
+          <t xml:space="preserve">Loss</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="H30">
+        <is>
+          <t xml:space="preserve">SIZE NOT SUITABLE</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="I30">
+        <is>
+          <t xml:space="preserve">SIZE TOO SMALL</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J30">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="K30">
+        <is>
+          <t xml:space="preserve">need big size</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="65">
+        <v>29</v>
+      </c>
+      <c t="inlineStr" r="B31">
+        <is>
+          <t xml:space="preserve">19-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C31">
+        <is>
+          <t xml:space="preserve">manu</t>
+        </is>
+      </c>
+      <c r="D31" s="65">
+        <v>8075300845</v>
+      </c>
+      <c t="inlineStr" r="E31">
+        <is>
+          <t xml:space="preserve">25-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F31">
+        <is>
+          <t xml:space="preserve">MUHAMMED ROSHAN C V</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G31">
+        <is>
+          <t xml:space="preserve">Loss</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="H31">
+        <is>
+          <t xml:space="preserve">ENQUIRY</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="I31">
+        <is>
+          <t xml:space="preserve">ENQUIRY WITHOUT BRIDE/FAMILY</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J31">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="K31">
+        <is>
+          <t xml:space="preserve">Revisit again with family</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="65">
+        <v>30</v>
+      </c>
+      <c t="inlineStr" r="B32">
+        <is>
+          <t xml:space="preserve">19-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C32">
+        <is>
+          <t xml:space="preserve">anshith</t>
+        </is>
+      </c>
+      <c r="D32" s="65">
+        <v>8129285123</v>
+      </c>
+      <c t="inlineStr" r="E32">
+        <is>
+          <t xml:space="preserve">22-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F32">
+        <is>
+          <t xml:space="preserve">MUHAMMED ROSHAN C V</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G32">
+        <is>
+          <t xml:space="preserve">Loss</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="H32">
+        <is>
+          <t xml:space="preserve">PRICING</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="I32">
+        <is>
+          <t xml:space="preserve">RENT TO HIGH</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J32">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="K32">
+        <is>
+          <t xml:space="preserve">price issue</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="65">
+        <v>31</v>
+      </c>
+      <c t="inlineStr" r="B33">
+        <is>
+          <t xml:space="preserve">19-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C33">
+        <is>
+          <t xml:space="preserve">raishad</t>
+        </is>
+      </c>
+      <c r="D33" s="65">
+        <v>9645779686</v>
+      </c>
+      <c t="inlineStr" r="E33">
+        <is>
+          <t xml:space="preserve">20-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F33">
+        <is>
+          <t xml:space="preserve">MUHAMMED ROSHAN C V</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G33">
+        <is>
+          <t xml:space="preserve">Loss</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="H33">
+        <is>
+          <t xml:space="preserve">ENQUIRY</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="I33">
+        <is>
+          <t xml:space="preserve">Enquiry for Relative/Friend</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J33">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="K33">
+        <is>
+          <t xml:space="preserve">Need to visit other stores</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="65">
+        <v>32</v>
+      </c>
+      <c t="inlineStr" r="B34">
+        <is>
+          <t xml:space="preserve">20-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C34">
+        <is>
+          <t xml:space="preserve">musthaq</t>
+        </is>
+      </c>
+      <c r="D34" s="65">
+        <v>8606453675</v>
+      </c>
+      <c t="inlineStr" r="E34">
+        <is>
+          <t xml:space="preserve">24-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F34">
+        <is>
+          <t xml:space="preserve">AKHIL K</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G34">
+        <is>
+          <t xml:space="preserve">Loss</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="H34">
+        <is>
+          <t xml:space="preserve">SIZE NOT SUITABLE</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="I34">
+        <is>
+          <t xml:space="preserve">SIZE TOO LARGE</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J34">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="K34">
+        <is>
+          <t xml:space="preserve">NEED BIG SIZE</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="65">
+        <v>33</v>
+      </c>
+      <c t="inlineStr" r="B35">
+        <is>
+          <t xml:space="preserve">20-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C35">
+        <is>
+          <t xml:space="preserve">Dani</t>
+        </is>
+      </c>
+      <c r="D35" s="65">
+        <v>8884829006</v>
+      </c>
+      <c t="inlineStr" r="E35">
+        <is>
+          <t xml:space="preserve">03-01-2026</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F35">
+        <is>
+          <t xml:space="preserve">AKHIL K</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G35">
+        <is>
+          <t xml:space="preserve">Loss</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="H35">
+        <is>
+          <t xml:space="preserve">ENQUIRY</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="I35">
+        <is>
+          <t xml:space="preserve">ENQUIRY WITHOUT BRIDE/FAMILY</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J35">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="K35">
+        <is>
+          <t xml:space="preserve">revisit with family</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="65">
+        <v>34</v>
+      </c>
+      <c t="inlineStr" r="B36">
+        <is>
+          <t xml:space="preserve">20-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C36">
+        <is>
+          <t xml:space="preserve">arshad</t>
+        </is>
+      </c>
+      <c r="D36" s="65">
+        <v>9495455949</v>
+      </c>
+      <c t="inlineStr" r="E36">
+        <is>
+          <t xml:space="preserve">04-01-2026</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F36">
+        <is>
+          <t xml:space="preserve">AKHIL K</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G36">
+        <is>
+          <t xml:space="preserve">Loss</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="H36">
+        <is>
+          <t xml:space="preserve">CUSTOMER INTERNAL ISSUES</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="I36">
+        <is>
+          <t xml:space="preserve">FAMILY DISAPPROVEL</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J36">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="K36">
+        <is>
+          <t xml:space="preserve">WILL REVISIT WITH FAMILY</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="65">
+        <v>35</v>
+      </c>
+      <c t="inlineStr" r="B37">
+        <is>
+          <t xml:space="preserve">21-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C37">
+        <is>
+          <t xml:space="preserve">dishnu</t>
+        </is>
+      </c>
+      <c r="D37" s="65">
+        <v>9747956458</v>
+      </c>
+      <c t="inlineStr" r="E37">
+        <is>
+          <t xml:space="preserve">25-01-2026</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F37">
+        <is>
+          <t xml:space="preserve">MUHAMMED ROSHAN C V</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G37">
+        <is>
+          <t xml:space="preserve">Loss</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="H37">
+        <is>
+          <t xml:space="preserve">ENQUIRY</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="I37">
+        <is>
+          <t xml:space="preserve">ENQUIRY WITHOUT BRIDE/FAMILY</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J37">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="K37">
+        <is>
+          <t xml:space="preserve">will rivisit again</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="65">
+        <v>36</v>
+      </c>
+      <c t="inlineStr" r="B38">
+        <is>
+          <t xml:space="preserve">21-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C38">
+        <is>
+          <t xml:space="preserve">fariz</t>
+        </is>
+      </c>
+      <c r="D38" s="65">
+        <v>9745765774</v>
+      </c>
+      <c t="inlineStr" r="E38">
+        <is>
+          <t xml:space="preserve">26-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F38">
+        <is>
+          <t xml:space="preserve">AKHIL K</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G38">
+        <is>
+          <t xml:space="preserve">Loss</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="H38">
+        <is>
+          <t xml:space="preserve">PRODUCT</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="I38">
+        <is>
+          <t xml:space="preserve">PRODUCT NOT AVAILABLE</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J38">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="K38">
+        <is>
+          <t xml:space="preserve">kurta big size 46 above</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="65">
+        <v>37</v>
+      </c>
+      <c t="inlineStr" r="B39">
+        <is>
+          <t xml:space="preserve">21-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C39">
+        <is>
+          <t xml:space="preserve">Fasil</t>
+        </is>
+      </c>
+      <c r="D39" s="65">
+        <v>9846549345</v>
+      </c>
+      <c t="inlineStr" r="E39">
+        <is>
+          <t xml:space="preserve">26-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F39">
+        <is>
+          <t xml:space="preserve">AKHIL K</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G39">
+        <is>
+          <t xml:space="preserve">Loss</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="H39">
+        <is>
+          <t xml:space="preserve">PRODUCT</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="I39">
+        <is>
+          <t xml:space="preserve">REQUIRED MODEL NOT AVAILABLE</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J39">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="K39">
+        <is>
+          <t xml:space="preserve">design not okay</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="65">
+        <v>38</v>
+      </c>
+      <c t="inlineStr" r="B40">
+        <is>
+          <t xml:space="preserve">21-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C40">
+        <is>
+          <t xml:space="preserve">ashwin</t>
+        </is>
+      </c>
+      <c r="D40" s="65">
+        <v>7907654063</v>
+      </c>
+      <c t="inlineStr" r="E40">
+        <is>
+          <t xml:space="preserve">29-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F40">
+        <is>
+          <t xml:space="preserve">MUHAMMED ROSHAN C V</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G40">
+        <is>
+          <t xml:space="preserve">Loss</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="H40">
+        <is>
+          <t xml:space="preserve">ENQUIRY</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="I40">
+        <is>
+          <t xml:space="preserve">ENQUIRY WITHOUT BRIDE/FAMILY</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J40">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="K40">
+        <is>
+          <t xml:space="preserve">custumer need to visit other stores</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="65">
+        <v>39</v>
+      </c>
+      <c t="inlineStr" r="B41">
+        <is>
+          <t xml:space="preserve">21-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C41">
+        <is>
+          <t xml:space="preserve">midhun</t>
+        </is>
+      </c>
+      <c r="D41" s="65">
+        <v>8075389771</v>
+      </c>
+      <c t="inlineStr" r="E41">
+        <is>
+          <t xml:space="preserve">31-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F41">
+        <is>
+          <t xml:space="preserve">MUHAMMED ROSHAN C V</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G41">
+        <is>
+          <t xml:space="preserve">Loss</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="H41">
+        <is>
+          <t xml:space="preserve">ENQUIRY</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="I41">
+        <is>
+          <t xml:space="preserve">ENQUIRY WITHOUT BRIDE/FAMILY</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J41">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="K41">
+        <is>
+          <t xml:space="preserve">rivisit again</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="65">
+        <v>40</v>
+      </c>
+      <c t="inlineStr" r="B42">
+        <is>
+          <t xml:space="preserve">21-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C42">
+        <is>
+          <t xml:space="preserve">Nandhu</t>
+        </is>
+      </c>
+      <c r="D42" s="65">
+        <v>9987332165</v>
+      </c>
+      <c t="inlineStr" r="E42">
+        <is>
+          <t xml:space="preserve">28-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F42">
+        <is>
+          <t xml:space="preserve">AKHIL K</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G42">
+        <is>
+          <t xml:space="preserve">Loss</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="H42">
+        <is>
+          <t xml:space="preserve">ENQUIRY</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="I42">
+        <is>
+          <t xml:space="preserve">ENQUIRY WITHOUT BRIDE/FAMILY</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J42">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="K42">
+        <is>
+          <t xml:space="preserve">revisit again</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="65">
+        <v>41</v>
+      </c>
+      <c t="inlineStr" r="B43">
+        <is>
+          <t xml:space="preserve">21-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C43">
+        <is>
+          <t xml:space="preserve">mushtaq</t>
+        </is>
+      </c>
+      <c r="D43" s="65">
+        <v>9074584488</v>
+      </c>
+      <c t="inlineStr" r="E43">
+        <is>
+          <t xml:space="preserve">12-01-2026</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F43">
+        <is>
+          <t xml:space="preserve">AKHIL K</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G43">
+        <is>
+          <t xml:space="preserve">Loss</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="H43">
+        <is>
+          <t xml:space="preserve">ENQUIRY</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="I43">
+        <is>
+          <t xml:space="preserve">ENQUIRY WITHOUT TRIAL</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J43">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="K43">
+        <is>
+          <t xml:space="preserve">revisit January 12</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat(loss-of-sale): import new loss-of-sale data
- added newly received loss-of-sale records
- ensured data consistency with existing schema
- verified records are available for reporting and filtering
</commit_message>
<xml_diff>
--- a/data/lossofsale_sg_calicut.xlsx
+++ b/data/lossofsale_sg_calicut.xlsx
@@ -2451,6 +2451,324 @@
         </is>
       </c>
     </row>
+    <row r="44">
+      <c r="A44" s="65">
+        <v>42</v>
+      </c>
+      <c t="inlineStr" r="B44">
+        <is>
+          <t xml:space="preserve">22-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C44">
+        <is>
+          <t xml:space="preserve">varun</t>
+        </is>
+      </c>
+      <c r="D44" s="65">
+        <v>8289959250</v>
+      </c>
+      <c t="inlineStr" r="E44">
+        <is>
+          <t xml:space="preserve">05-01-2026</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F44">
+        <is>
+          <t xml:space="preserve">SHAIKRIZWAN</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G44">
+        <is>
+          <t xml:space="preserve">Loss</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="H44">
+        <is>
+          <t xml:space="preserve">PRODUCT</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="I44">
+        <is>
+          <t xml:space="preserve">REQUIRED MODEL NOT AVAILABLE</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J44">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="K44">
+        <is>
+          <t xml:space="preserve">NEED MINIMAL WORK</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="65">
+        <v>43</v>
+      </c>
+      <c t="inlineStr" r="B45">
+        <is>
+          <t xml:space="preserve">22-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C45">
+        <is>
+          <t xml:space="preserve">aparna</t>
+        </is>
+      </c>
+      <c r="D45" s="65">
+        <v>8590441298</v>
+      </c>
+      <c t="inlineStr" r="E45">
+        <is>
+          <t xml:space="preserve">23-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F45">
+        <is>
+          <t xml:space="preserve">MUHAMMED ROSHAN C V</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G45">
+        <is>
+          <t xml:space="preserve">Loss</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="H45">
+        <is>
+          <t xml:space="preserve">SIZE NOT SUITABLE</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="I45">
+        <is>
+          <t xml:space="preserve">SIZE TOO SMALL</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J45">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="K45">
+        <is>
+          <t xml:space="preserve">NEED BIG SIZE</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="65">
+        <v>44</v>
+      </c>
+      <c t="inlineStr" r="B46">
+        <is>
+          <t xml:space="preserve">22-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C46">
+        <is>
+          <t xml:space="preserve">ashwin</t>
+        </is>
+      </c>
+      <c r="D46" s="65">
+        <v>9061864064</v>
+      </c>
+      <c t="inlineStr" r="E46">
+        <is>
+          <t xml:space="preserve">01-02-2026</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F46">
+        <is>
+          <t xml:space="preserve">MUHAMMED ROSHAN C V</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G46">
+        <is>
+          <t xml:space="preserve">Loss</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="H46">
+        <is>
+          <t xml:space="preserve">ENQUIRY</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="I46">
+        <is>
+          <t xml:space="preserve">ENQUIRY WITHOUT BRIDE/FAMILY</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J46">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="K46">
+        <is>
+          <t xml:space="preserve">WILL REVISIT</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="65">
+        <v>45</v>
+      </c>
+      <c t="inlineStr" r="B47">
+        <is>
+          <t xml:space="preserve">23-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C47">
+        <is>
+          <t xml:space="preserve">Akash</t>
+        </is>
+      </c>
+      <c r="D47" s="65">
+        <v>9037331112</v>
+      </c>
+      <c t="inlineStr" r="E47">
+        <is>
+          <t xml:space="preserve">03-01-2026</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F47">
+        <is>
+          <t xml:space="preserve">MUHAMMED ROSHAN C V</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G47">
+        <is>
+          <t xml:space="preserve">Loss</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="H47">
+        <is>
+          <t xml:space="preserve">SIZE NOT SUITABLE</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="I47">
+        <is>
+          <t xml:space="preserve">SIZE TOO SMALL</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J47">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="K47">
+        <is>
+          <t xml:space="preserve">need bigger size IW</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="65">
+        <v>46</v>
+      </c>
+      <c t="inlineStr" r="B48">
+        <is>
+          <t xml:space="preserve">24-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C48">
+        <is>
+          <t xml:space="preserve">anuraj</t>
+        </is>
+      </c>
+      <c r="D48" s="65">
+        <v>8289893408</v>
+      </c>
+      <c t="inlineStr" r="E48">
+        <is>
+          <t xml:space="preserve">26-01-2026</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F48">
+        <is>
+          <t xml:space="preserve">SHAIKRIZWAN</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G48">
+        <is>
+          <t xml:space="preserve">Loss</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="H48">
+        <is>
+          <t xml:space="preserve">ENQUIRY</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="I48">
+        <is>
+          <t xml:space="preserve">ENQUIRY WITHOUT BRIDE/FAMILY</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J48">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="K48">
+        <is>
+          <t xml:space="preserve">need to visit our vadakara store</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="65">
+        <v>47</v>
+      </c>
+      <c t="inlineStr" r="B49">
+        <is>
+          <t xml:space="preserve">25-12-2025</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="C49">
+        <is>
+          <t xml:space="preserve">arjun</t>
+        </is>
+      </c>
+      <c r="D49" s="65">
+        <v>9544974956</v>
+      </c>
+      <c t="inlineStr" r="E49">
+        <is>
+          <t xml:space="preserve">04-01-2026</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="F49">
+        <is>
+          <t xml:space="preserve">MUHAMMED ROSHAN C V</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="G49">
+        <is>
+          <t xml:space="preserve">Loss</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="H49">
+        <is>
+          <t xml:space="preserve">ENQUIRY</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="I49">
+        <is>
+          <t xml:space="preserve">ENQUIRY WITHOUT BRIDE/FAMILY</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J49">
+        <is>
+          <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="K49">
+        <is>
+          <t xml:space="preserve">need to visit other store</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:K1"/>

</xml_diff>